<commit_message>
add comment in fencei vplan about flush
Signed-off-by: Robin Pedersen <Robin.Pedersen@silabs.com>
</commit_message>
<xml_diff>
--- a/cv32e40s/docs/VerifPlans/Simulation/micro_architecture/CV32E40SX_fencei.xlsx
+++ b/cv32e40s/docs/VerifPlans/Simulation/micro_architecture/CV32E40SX_fencei.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ropeders\Documents\fencei_vplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2586A5-9422-4498-B2C2-01ABC1614E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25BCE84-57F3-42E4-950C-32ACB6363148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="High-level Feature" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="120">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -332,9 +332,6 @@
   <si>
     <t>A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.fencei_assert_i.a_req_stay_high
 A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.fencei_assert_i.a_req_drop_lo</t>
-  </si>
-  <si>
-    <t>A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.fencei_assert_i.a_supress_datareq</t>
   </si>
   <si>
     <t>Given zero stalls on neither instr-side and data-side obi nor on fencei_flush_ack_i, then the execution of fence.i takes a fixed number of cycles.</t>
@@ -394,6 +391,13 @@
   </si>
   <si>
     <t>TODO missing assert. (Note was ignored because of the difficulty of writing this as an assert for fv.)</t>
+  </si>
+  <si>
+    <t>A: uvmt_cv32e40s_tb.dut_wrap.cv32e40s_wrapper_i.fencei_assert_i.a_supress_datareq
+A: ???</t>
+  </si>
+  <si>
+    <t>TODO missing assert. (Have not checked/covered that the pipeline/writebuffer content is actually purged. Or that any memory change WILL be the next instr word.)</t>
   </si>
 </sst>
 </file>
@@ -505,14 +509,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -898,10 +902,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMJ36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -920,565 +924,568 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="J14" s="12"/>
+    </row>
+    <row r="15" spans="1:10" customFormat="1" ht="151.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" customFormat="1" ht="179.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="J20" s="12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:10" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="J3" s="13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" customFormat="1" ht="69" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="J8" s="13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" customFormat="1" ht="69" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" customFormat="1" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="J10" s="13"/>
-    </row>
-    <row r="11" spans="1:10" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" customFormat="1" ht="69" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" customFormat="1" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="J14" s="13"/>
-    </row>
-    <row r="15" spans="1:10" customFormat="1" ht="157.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="13" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H19" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" customFormat="1" ht="73.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" customFormat="1" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1489,7 +1496,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1500,7 +1507,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1511,7 +1518,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1522,7 +1529,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1533,7 +1540,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1544,7 +1551,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1555,7 +1562,7 @@
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1566,7 +1573,7 @@
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1577,7 +1584,7 @@
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1588,7 +1595,7 @@
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1633,17 +1640,17 @@
       <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>